<commit_message>
adding sprint 2 burndown report
</commit_message>
<xml_diff>
--- a/Sprint 2 Burndown.xlsx
+++ b/Sprint 2 Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Development\team-b3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A6EDB55-ADC7-402E-85FE-EEEDF47FE0F6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E3F0E79-6583-4D4E-827A-456FBF21531F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6850" xr2:uid="{2A4C6EDA-AF40-4229-894C-6BC58B2B9163}"/>
   </bookViews>
@@ -1380,7 +1380,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77206CDB-DD11-4F6F-B110-DF011E1F14CB}">
   <dimension ref="B2:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>